<commit_message>
New column: alamat, pdf file fixes
</commit_message>
<xml_diff>
--- a/uploads/excel/userfile.xlsx
+++ b/uploads/excel/userfile.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fudi\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\webpetra-master\uploads\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5173CF52-63EF-4800-BFE5-BA0C346A7453}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="15375" windowHeight="8325" xr2:uid="{B66F9D8A-D6FE-4274-9B46-D459B5F8A7BC}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="15375" windowHeight="8325"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="26">
   <si>
     <t>1/1/1/1</t>
   </si>
@@ -48,18 +47,12 @@
     <t>pastor4</t>
   </si>
   <si>
-    <t>001_GPT_A_V_19</t>
-  </si>
-  <si>
     <t>1/1/1/2</t>
   </si>
   <si>
     <t>pastor5</t>
   </si>
   <si>
-    <t>001_GPT_A_V_20</t>
-  </si>
-  <si>
     <t>1/1/1/3</t>
   </si>
   <si>
@@ -87,57 +80,36 @@
     <t>pastor6</t>
   </si>
   <si>
-    <t>001_GPT_A_V_21</t>
-  </si>
-  <si>
     <t>pastor7</t>
   </si>
   <si>
-    <t>001_GPT_A_V_22</t>
-  </si>
-  <si>
     <t>pastor8</t>
   </si>
   <si>
-    <t>001_GPT_A_V_23</t>
-  </si>
-  <si>
     <t>pastor9</t>
   </si>
   <si>
-    <t>001_GPT_A_V_24</t>
-  </si>
-  <si>
     <t>pastor10</t>
   </si>
   <si>
-    <t>001_GPT_A_V_25</t>
-  </si>
-  <si>
     <t>pastor11</t>
   </si>
   <si>
-    <t>001_GPT_A_V_26</t>
-  </si>
-  <si>
     <t>pastor12</t>
   </si>
   <si>
-    <t>001_GPT_A_V_27</t>
-  </si>
-  <si>
     <t>pastor13</t>
   </si>
   <si>
-    <t>001_GPT_A_V_28</t>
+    <t>alamatku</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -170,7 +142,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,17 +456,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4837F2-1E9E-4DC6-AB0B-8616FA557DE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D10"/>
+      <selection activeCell="K1" sqref="K1:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -511,27 +483,27 @@
         <v>33095</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1">
         <v>26399</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -543,27 +515,27 @@
         <v>33096</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1">
         <v>26400</v>
       </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
       <c r="J2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -575,27 +547,27 @@
         <v>33097</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="1">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1">
         <v>26401</v>
       </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
       <c r="J3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -607,27 +579,27 @@
         <v>33098</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="1">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
         <v>26402</v>
       </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -639,27 +611,27 @@
         <v>33099</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="1">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1">
         <v>26403</v>
       </c>
-      <c r="I5" t="s">
-        <v>23</v>
-      </c>
       <c r="J5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -671,27 +643,27 @@
         <v>33100</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="1">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1">
         <v>26404</v>
       </c>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -703,27 +675,27 @@
         <v>33101</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="1">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="1">
         <v>26405</v>
       </c>
-      <c r="I7" t="s">
-        <v>27</v>
-      </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -735,27 +707,27 @@
         <v>33102</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="1">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1">
         <v>26406</v>
       </c>
-      <c r="I8" t="s">
-        <v>29</v>
-      </c>
       <c r="J8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -767,27 +739,27 @@
         <v>33103</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="1">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="1">
         <v>26407</v>
       </c>
-      <c r="I9" t="s">
-        <v>31</v>
-      </c>
       <c r="J9" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -799,22 +771,22 @@
         <v>33104</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="1">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="1">
         <v>26408</v>
       </c>
-      <c r="I10" t="s">
-        <v>33</v>
-      </c>
       <c r="J10" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>